<commit_message>
update method to seekFiles
</commit_message>
<xml_diff>
--- a/bin/Debug/net8.0/results.xlsx
+++ b/bin/Debug/net8.0/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t xml:space="preserve">Path</t>
   </si>
@@ -24,6 +24,51 @@
   </si>
   <si>
     <t xml:space="preserve">Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\competences.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File not found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\experiences.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\loisirs.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\img\testfile\test\Nouveau document texte - Copie (2).txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\img\testfile\test\Nouveau document texte - Copie (3).txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\img\testfile\test\Nouveau document texte - Copie (4).txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\img\testfile\test\Nouveau document texte - Copie (5).txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\img\testfile\test\Nouveau document texte - Copie.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\img\testfile\test\Nouveau document texte.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\img\testfile\test\tezst\Nouveau document texte - Copie (2).txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\img\testfile\test\tezst\Nouveau document texte - Copie (3).txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\img\testfile\test\tezst\Nouveau document texte - Copie.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D:\AProg\html\PortfolioC\img\testfile\test\tezst\Nouveau document texte.txt</t>
   </si>
 </sst>
 </file>
@@ -295,6 +340,188 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="default"/>

</xml_diff>